<commit_message>
fix for tables query to .xlsx
</commit_message>
<xml_diff>
--- a/test_workbook.xlsx
+++ b/test_workbook.xlsx
@@ -7,8 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="answers" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="answers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="hospitals" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="icu_beds_available" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="patient_responses" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="patients" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="questions" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +21,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,8 +53,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -346,19 +353,263 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>question_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>answers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>hospital_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>total_icu_beds</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>total_vents</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>working_vents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>latitutde</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>hospital_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>beds_in_use</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>vents_in_use</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>recorded_at</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>43932.11472222222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>patient_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>question_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>answer_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>recorded_at</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>hospital_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>patient_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>patient_mr_no</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>entry_point</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>recorded_at</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -380,12 +631,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>question_id</t>
+          <t>question</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>answers</t>
+          <t>question_type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">

</xml_diff>